<commit_message>
add new methods in calss ressurealculationodel
</commit_message>
<xml_diff>
--- a/output/results/model_parameters.xlsx
+++ b/output/results/model_parameters.xlsx
@@ -647,7 +647,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1679524210452392</v>
+        <v>0.2360754472511452</v>
       </c>
     </row>
     <row r="3">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2377598023895837</v>
+        <v>0.06526393968409917</v>
       </c>
     </row>
     <row r="4">
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5309436823749749</v>
+        <v>0.1864554834859687</v>
       </c>
     </row>
     <row r="5">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2329282749436502</v>
+        <v>0.5016168286296921</v>
       </c>
     </row>
   </sheetData>
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-2.754007093465581</v>
+        <v>-2.929461255352919</v>
       </c>
     </row>
     <row r="3">
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.3094818668944162</v>
+        <v>0.07729346639100185</v>
       </c>
     </row>
     <row r="4">
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01245280595218202</v>
+        <v>0.009714626772967951</v>
       </c>
     </row>
   </sheetData>
@@ -779,7 +779,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.996938132450026</v>
+        <v>1.008068653043437</v>
       </c>
     </row>
     <row r="3">
@@ -789,7 +789,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4783483911785228</v>
+        <v>0.5342636214790784</v>
       </c>
     </row>
     <row r="4">
@@ -799,7 +799,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.002873939925204812</v>
+        <v>0.003706813271053893</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +840,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3.524930189558297</v>
+        <v>3.846026467336558</v>
       </c>
     </row>
     <row r="3">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3233100660226062</v>
+        <v>0.3181181968665893</v>
       </c>
     </row>
     <row r="4">
@@ -860,7 +860,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4385947536294357</v>
+        <v>0.637621805276343</v>
       </c>
     </row>
     <row r="5">
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.02019871684509267</v>
+        <v>0.02693643592064818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>